<commit_message>
Minor changes during submission.
</commit_message>
<xml_diff>
--- a/data/SuppTable3__SouthAfrica_ONT-vs-Illumina_metadata.xlsx
+++ b/data/SuppTable3__SouthAfrica_ONT-vs-Illumina_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb29/Papers/AmpliSeq_Treponema_paper_2024/Github/TP-Phylo-Plex_paper_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E8E2A-90AC-8545-BAC6-FF3FC5A88330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5687907C-AAE7-FB4D-A377-F540ED9B431F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="28800" windowHeight="14520" xr2:uid="{7D288DAB-841B-5641-863B-83446A7A6A09}"/>
+    <workbookView xWindow="-33580" yWindow="2840" windowWidth="28800" windowHeight="14520" xr2:uid="{7D288DAB-841B-5641-863B-83446A7A6A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="486">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1496,6 +1496,9 @@
   </si>
   <si>
     <t>ONT-reads-still-not-online-yet</t>
+  </si>
+  <si>
+    <t>tbd</t>
   </si>
 </sst>
 </file>
@@ -1923,7 +1926,7 @@
   <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2970,8 +2973,8 @@
       <c r="G18" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="7" t="e">
-        <v>#N/A</v>
+      <c r="H18" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="I18" s="1">
         <v>3.6</v>
@@ -3855,8 +3858,8 @@
       <c r="G33" t="s">
         <v>107</v>
       </c>
-      <c r="H33" s="7" t="e">
-        <v>#N/A</v>
+      <c r="H33" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="I33" s="1">
         <v>3.3</v>
@@ -4386,8 +4389,8 @@
       <c r="G42" t="s">
         <v>116</v>
       </c>
-      <c r="H42" s="7" t="e">
-        <v>#N/A</v>
+      <c r="H42" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="I42" s="1">
         <v>3.72</v>
@@ -4504,8 +4507,8 @@
       <c r="G44" t="s">
         <v>118</v>
       </c>
-      <c r="H44" s="7" t="e">
-        <v>#N/A</v>
+      <c r="H44" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="I44" s="1">
         <v>2.84</v>
@@ -4622,8 +4625,8 @@
       <c r="G46" t="s">
         <v>120</v>
       </c>
-      <c r="H46" s="7" t="e">
-        <v>#N/A</v>
+      <c r="H46" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="I46" s="1">
         <v>2.46</v>

</xml_diff>